<commit_message>
[Update] Final touches before hand-in
</commit_message>
<xml_diff>
--- a/docs/[TC] Buy Ticket.xlsx
+++ b/docs/[TC] Buy Ticket.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eclipse Workspace\PayStation\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1134421-7742-4157-BEE9-3819979BC308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19574C7-5159-47FC-BB89-4BDA2DD495DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="0" windowWidth="16725" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -372,7 +372,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -470,6 +470,66 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -479,80 +539,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -840,7 +843,7 @@
   <dimension ref="B1:U44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N9"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,49 +865,49 @@
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.25">
       <c r="N1" s="15"/>
-      <c r="O1" s="47" t="s">
+      <c r="O1" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
     </row>
     <row r="2" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="41" t="s">
+      <c r="B2" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="45" t="s">
+      <c r="J2" s="54"/>
+      <c r="K2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="46"/>
-      <c r="M2" s="41" t="s">
+      <c r="L2" s="59"/>
+      <c r="M2" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="54" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="40"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
@@ -923,23 +926,23 @@
       <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="K3" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="42" t="s">
+      <c r="L3" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
     </row>
     <row r="4" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="40"/>
+      <c r="B4" s="63"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -958,12 +961,12 @@
       <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
     </row>
     <row r="5" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="9">
@@ -999,7 +1002,7 @@
       <c r="L5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="48" t="s">
+      <c r="M5" s="50" t="s">
         <v>29</v>
       </c>
       <c r="N5" s="21"/>
@@ -1037,64 +1040,64 @@
       <c r="L6" s="4">
         <v>0</v>
       </c>
-      <c r="M6" s="49"/>
+      <c r="M6" s="52"/>
       <c r="N6" s="23"/>
     </row>
     <row r="7" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="13">
         <v>2</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="62">
         <v>5</v>
       </c>
-      <c r="D7" s="44">
-        <v>0</v>
-      </c>
-      <c r="E7" s="44">
-        <v>0</v>
-      </c>
-      <c r="F7" s="44">
-        <v>0</v>
-      </c>
-      <c r="G7" s="44">
-        <v>0</v>
-      </c>
-      <c r="H7" s="44">
-        <v>0</v>
-      </c>
-      <c r="I7" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" s="48" t="s">
+      <c r="D7" s="62">
+        <v>0</v>
+      </c>
+      <c r="E7" s="62">
+        <v>0</v>
+      </c>
+      <c r="F7" s="62">
+        <v>0</v>
+      </c>
+      <c r="G7" s="62">
+        <v>0</v>
+      </c>
+      <c r="H7" s="62">
+        <v>0</v>
+      </c>
+      <c r="I7" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="35"/>
+      <c r="N7" s="55"/>
     </row>
     <row r="8" spans="2:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="36"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="56"/>
     </row>
     <row r="9" spans="2:21" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
@@ -1125,10 +1128,14 @@
         <f>_xlfn.CEILING.MATH(I9/60)</f>
         <v>2</v>
       </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="37"/>
+      <c r="K9" s="35">
+        <v>120</v>
+      </c>
+      <c r="L9" s="1">
+        <v>2</v>
+      </c>
+      <c r="M9" s="52"/>
+      <c r="N9" s="57"/>
     </row>
     <row r="10" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
@@ -1164,7 +1171,7 @@
       <c r="L10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="51"/>
+      <c r="M10" s="36"/>
       <c r="N10" s="21"/>
     </row>
     <row r="11" spans="2:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -1201,7 +1208,7 @@
       <c r="L11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M11" s="52" t="s">
+      <c r="M11" s="37" t="s">
         <v>29</v>
       </c>
       <c r="N11" s="22"/>
@@ -1235,9 +1242,11 @@
         <f>I12/60</f>
         <v>120</v>
       </c>
-      <c r="K12" s="4"/>
+      <c r="K12" s="4">
+        <v>7200</v>
+      </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="53"/>
+      <c r="M12" s="38"/>
       <c r="N12" s="23"/>
     </row>
     <row r="13" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1266,7 +1275,7 @@
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
-      <c r="M13" s="48" t="s">
+      <c r="M13" s="50" t="s">
         <v>29</v>
       </c>
       <c r="N13" s="18"/>
@@ -1285,7 +1294,7 @@
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
-      <c r="M14" s="50"/>
+      <c r="M14" s="51"/>
       <c r="N14" s="19"/>
     </row>
     <row r="15" spans="2:21" ht="47.25" x14ac:dyDescent="0.25">
@@ -1305,11 +1314,13 @@
         <f>_xlfn.CEILING.MATH(I15/60)</f>
         <v>27</v>
       </c>
-      <c r="K15" s="3"/>
+      <c r="K15" s="3">
+        <v>1600</v>
+      </c>
       <c r="L15" s="3">
         <v>27</v>
       </c>
-      <c r="M15" s="49"/>
+      <c r="M15" s="52"/>
       <c r="N15" s="20"/>
     </row>
     <row r="16" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1338,7 +1349,7 @@
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
-      <c r="M16" s="48" t="s">
+      <c r="M16" s="50" t="s">
         <v>29</v>
       </c>
       <c r="N16" s="21"/>
@@ -1357,7 +1368,7 @@
       <c r="J17" s="29"/>
       <c r="K17" s="29"/>
       <c r="L17" s="29"/>
-      <c r="M17" s="50"/>
+      <c r="M17" s="51"/>
       <c r="N17" s="22"/>
     </row>
     <row r="18" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1384,7 +1395,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="50"/>
+      <c r="M18" s="51"/>
       <c r="N18" s="22"/>
     </row>
     <row r="19" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1404,9 +1415,13 @@
         <f>_xlfn.CEILING.MATH(I19/60)</f>
         <v>160</v>
       </c>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="49"/>
+      <c r="K19" s="5">
+        <v>9600</v>
+      </c>
+      <c r="L19" s="5">
+        <v>160</v>
+      </c>
+      <c r="M19" s="52"/>
       <c r="N19" s="23"/>
     </row>
     <row r="20" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1435,7 +1450,7 @@
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
-      <c r="M20" s="48" t="s">
+      <c r="M20" s="50" t="s">
         <v>29</v>
       </c>
       <c r="N20" s="18"/>
@@ -1454,7 +1469,7 @@
       <c r="J21" s="17"/>
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
-      <c r="M21" s="50"/>
+      <c r="M21" s="51"/>
       <c r="N21" s="19"/>
     </row>
     <row r="22" spans="2:14" ht="47.25" x14ac:dyDescent="0.25">
@@ -1486,9 +1501,13 @@
         <f>_xlfn.CEILING.MATH(I22/60)</f>
         <v>107</v>
       </c>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="49"/>
+      <c r="K22" s="3">
+        <v>6400</v>
+      </c>
+      <c r="L22" s="3">
+        <v>107</v>
+      </c>
+      <c r="M22" s="52"/>
       <c r="N22" s="20"/>
     </row>
     <row r="23" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1517,7 +1536,7 @@
       <c r="J23" s="28"/>
       <c r="K23" s="28"/>
       <c r="L23" s="28"/>
-      <c r="M23" s="48" t="s">
+      <c r="M23" s="50" t="s">
         <v>29</v>
       </c>
       <c r="N23" s="21"/>
@@ -1536,7 +1555,7 @@
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
       <c r="L24" s="29"/>
-      <c r="M24" s="50"/>
+      <c r="M24" s="51"/>
       <c r="N24" s="22"/>
     </row>
     <row r="25" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1563,7 +1582,7 @@
       <c r="J25" s="29"/>
       <c r="K25" s="29"/>
       <c r="L25" s="29"/>
-      <c r="M25" s="50"/>
+      <c r="M25" s="51"/>
       <c r="N25" s="22"/>
     </row>
     <row r="26" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1590,7 +1609,7 @@
       <c r="J26" s="29"/>
       <c r="K26" s="29"/>
       <c r="L26" s="29"/>
-      <c r="M26" s="50"/>
+      <c r="M26" s="51"/>
       <c r="N26" s="22"/>
     </row>
     <row r="27" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1617,7 +1636,7 @@
       <c r="J27" s="29"/>
       <c r="K27" s="29"/>
       <c r="L27" s="29"/>
-      <c r="M27" s="50"/>
+      <c r="M27" s="51"/>
       <c r="N27" s="22"/>
     </row>
     <row r="28" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1644,7 +1663,7 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
-      <c r="M28" s="50"/>
+      <c r="M28" s="51"/>
       <c r="N28" s="22"/>
     </row>
     <row r="29" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
@@ -1664,9 +1683,13 @@
         <f>_xlfn.CEILING.MATH(I29/60)</f>
         <v>220</v>
       </c>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="49"/>
+      <c r="K29" s="5">
+        <v>13200</v>
+      </c>
+      <c r="L29" s="5">
+        <v>220</v>
+      </c>
+      <c r="M29" s="52"/>
       <c r="N29" s="23"/>
     </row>
     <row r="30" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1695,10 +1718,10 @@
       <c r="J30" s="25"/>
       <c r="K30" s="16"/>
       <c r="L30" s="16"/>
-      <c r="M30" s="48" t="s">
+      <c r="M30" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="N30" s="57"/>
+      <c r="N30" s="46"/>
     </row>
     <row r="31" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
@@ -1714,8 +1737,8 @@
       <c r="J31" s="27"/>
       <c r="K31" s="17"/>
       <c r="L31" s="17"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="58"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="47"/>
     </row>
     <row r="32" spans="2:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
@@ -1727,16 +1750,16 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="38" t="s">
+      <c r="I32" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="J32" s="39"/>
-      <c r="K32" s="38" t="s">
+      <c r="J32" s="40"/>
+      <c r="K32" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="L32" s="39"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="59"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="52"/>
+      <c r="N32" s="48"/>
     </row>
     <row r="33" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="9">
@@ -1764,10 +1787,10 @@
       <c r="J33" s="31"/>
       <c r="K33" s="28"/>
       <c r="L33" s="28"/>
-      <c r="M33" s="48" t="s">
+      <c r="M33" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="N33" s="60"/>
+      <c r="N33" s="49"/>
     </row>
     <row r="34" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="s">
@@ -1783,8 +1806,8 @@
       <c r="J34" s="33"/>
       <c r="K34" s="29"/>
       <c r="L34" s="29"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="61"/>
+      <c r="M34" s="51"/>
+      <c r="N34" s="44"/>
     </row>
     <row r="35" spans="2:14" ht="63" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
@@ -1796,16 +1819,16 @@
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="38" t="s">
+      <c r="I35" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="39"/>
-      <c r="K35" s="38" t="s">
+      <c r="J35" s="40"/>
+      <c r="K35" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="L35" s="39"/>
-      <c r="M35" s="49"/>
-      <c r="N35" s="62"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="45"/>
     </row>
     <row r="36" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="6">
@@ -1833,10 +1856,10 @@
       <c r="J36" s="25"/>
       <c r="K36" s="16"/>
       <c r="L36" s="16"/>
-      <c r="M36" s="48" t="s">
+      <c r="M36" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="N36" s="57"/>
+      <c r="N36" s="46"/>
     </row>
     <row r="37" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
@@ -1852,8 +1875,8 @@
       <c r="J37" s="27"/>
       <c r="K37" s="17"/>
       <c r="L37" s="17"/>
-      <c r="M37" s="50"/>
-      <c r="N37" s="58"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="47"/>
     </row>
     <row r="38" spans="2:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
@@ -1865,16 +1888,16 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="38" t="s">
+      <c r="I38" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="J38" s="39"/>
-      <c r="K38" s="38" t="s">
+      <c r="J38" s="40"/>
+      <c r="K38" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="L38" s="39"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="59"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="52"/>
+      <c r="N38" s="48"/>
     </row>
     <row r="39" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="9">
@@ -1902,7 +1925,7 @@
       <c r="J39" s="31"/>
       <c r="K39" s="28"/>
       <c r="L39" s="28"/>
-      <c r="M39" s="48" t="s">
+      <c r="M39" s="50" t="s">
         <v>29</v>
       </c>
       <c r="N39" s="21"/>
@@ -1921,8 +1944,8 @@
       <c r="J40" s="33"/>
       <c r="K40" s="29"/>
       <c r="L40" s="29"/>
-      <c r="M40" s="50"/>
-      <c r="N40" s="61"/>
+      <c r="M40" s="51"/>
+      <c r="N40" s="44"/>
     </row>
     <row r="41" spans="2:14" ht="63" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
@@ -1934,16 +1957,16 @@
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
-      <c r="I41" s="38" t="s">
+      <c r="I41" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="J41" s="39"/>
-      <c r="K41" s="38" t="s">
+      <c r="J41" s="40"/>
+      <c r="K41" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="L41" s="39"/>
-      <c r="M41" s="49"/>
-      <c r="N41" s="62"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="52"/>
+      <c r="N41" s="45"/>
     </row>
     <row r="42" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="6">
@@ -1971,10 +1994,10 @@
       <c r="J42" s="25"/>
       <c r="K42" s="16"/>
       <c r="L42" s="16"/>
-      <c r="M42" s="48" t="s">
+      <c r="M42" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="N42" s="54" t="s">
+      <c r="N42" s="41" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1992,8 +2015,8 @@
       <c r="J43" s="27"/>
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
-      <c r="M43" s="50"/>
-      <c r="N43" s="55"/>
+      <c r="M43" s="51"/>
+      <c r="N43" s="42"/>
     </row>
     <row r="44" spans="2:14" ht="63" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="s">
@@ -2005,29 +2028,49 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="38" t="s">
+      <c r="I44" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="J44" s="39"/>
-      <c r="K44" s="38" t="s">
+      <c r="J44" s="40"/>
+      <c r="K44" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="L44" s="39"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="56"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="52"/>
+      <c r="N44" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="N42:N44"/>
-    <mergeCell ref="N40:N41"/>
-    <mergeCell ref="N36:N38"/>
-    <mergeCell ref="N33:N35"/>
-    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="M13:M15"/>
+    <mergeCell ref="M16:M19"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="M23:M29"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="O1:U1"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="M5:M6"/>
     <mergeCell ref="M39:M41"/>
     <mergeCell ref="M42:M44"/>
     <mergeCell ref="I38:J38"/>
@@ -2038,36 +2081,16 @@
     <mergeCell ref="M30:M32"/>
     <mergeCell ref="M33:M35"/>
     <mergeCell ref="M36:M38"/>
-    <mergeCell ref="O1:U1"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M13:M15"/>
-    <mergeCell ref="M16:M19"/>
-    <mergeCell ref="M20:M22"/>
-    <mergeCell ref="M23:M29"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="N42:N44"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="N36:N38"/>
+    <mergeCell ref="N33:N35"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K35:L35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>